<commit_message>
Se arreglan datos 2022 y se actualizan gráficos
</commit_message>
<xml_diff>
--- a/Implementación/Indicadores demográficos INEC.xlsx
+++ b/Implementación/Indicadores demográficos INEC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peanuts\Documents\GitHub\Proyecto-SP-1357\Implementación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65B5AED-3B78-4B38-AEC4-A1F27F6E279F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A713B662-FD59-4584-9B37-675B1163ADEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="6" xr2:uid="{E147D909-6B07-4350-BE0A-080132B287DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{E147D909-6B07-4350-BE0A-080132B287DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos nom res." sheetId="5" r:id="rId1"/>
@@ -1071,10 +1071,40 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1092,37 +1122,7 @@
     <xf numFmtId="2" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -30316,8 +30316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D811B041-15C7-4C90-9BD8-AAE8AE4FD967}">
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AE1048576"/>
+    <sheetView topLeftCell="P24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -36856,16 +36856,36 @@
       <c r="Q74" s="66">
         <v>0.63</v>
       </c>
-      <c r="R74" s="62"/>
-      <c r="S74" s="62"/>
-      <c r="T74" s="62"/>
-      <c r="U74" s="62"/>
-      <c r="V74" s="48"/>
-      <c r="W74" s="48"/>
-      <c r="X74" s="48"/>
-      <c r="Y74" s="48"/>
-      <c r="Z74" s="48"/>
-      <c r="AA74" s="48"/>
+      <c r="R74" s="48">
+        <v>560</v>
+      </c>
+      <c r="S74" s="48">
+        <v>51</v>
+      </c>
+      <c r="T74" s="48">
+        <v>354</v>
+      </c>
+      <c r="U74" s="48">
+        <v>82</v>
+      </c>
+      <c r="V74" s="48">
+        <v>0.11719857428222107</v>
+      </c>
+      <c r="W74" s="48">
+        <v>0.21333422730533347</v>
+      </c>
+      <c r="X74" s="48">
+        <v>1.970340579164228E-2</v>
+      </c>
+      <c r="Y74" s="48">
+        <v>8.3631061189931896E-2</v>
+      </c>
+      <c r="Z74" s="48">
+        <v>0.13485770797515723</v>
+      </c>
+      <c r="AA74" s="48">
+        <v>3.167998578264053E-2</v>
+      </c>
       <c r="AB74" s="61">
         <v>22920</v>
       </c>
@@ -36897,10 +36917,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25">
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="98"/>
+      <c r="D1" s="82"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="69" t="s">
@@ -37093,10 +37113,10 @@
       <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="D15" s="97" t="s">
+      <c r="D15" s="81" t="s">
         <v>157</v>
       </c>
     </row>
@@ -37336,7 +37356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354E2676-582E-4F72-9DE7-4CD19FD089B4}">
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O40" workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -43871,16 +43893,36 @@
       <c r="Q74" s="66">
         <v>0.63</v>
       </c>
-      <c r="R74" s="62"/>
-      <c r="S74" s="62"/>
-      <c r="T74" s="62"/>
-      <c r="U74" s="62"/>
-      <c r="V74" s="48"/>
-      <c r="W74" s="48"/>
-      <c r="X74" s="48"/>
-      <c r="Y74" s="48"/>
-      <c r="Z74" s="48"/>
-      <c r="AA74" s="48"/>
+      <c r="R74" s="48">
+        <v>560</v>
+      </c>
+      <c r="S74" s="48">
+        <v>51</v>
+      </c>
+      <c r="T74" s="48">
+        <v>354</v>
+      </c>
+      <c r="U74" s="48">
+        <v>82</v>
+      </c>
+      <c r="V74" s="48">
+        <v>0.11719857428222107</v>
+      </c>
+      <c r="W74" s="48">
+        <v>0.21333422730533347</v>
+      </c>
+      <c r="X74" s="48">
+        <v>1.970340579164228E-2</v>
+      </c>
+      <c r="Y74" s="48">
+        <v>8.3631061189931896E-2</v>
+      </c>
+      <c r="Z74" s="48">
+        <v>0.13485770797515723</v>
+      </c>
+      <c r="AA74" s="48">
+        <v>3.167998578264053E-2</v>
+      </c>
       <c r="AB74" s="61">
         <v>22920</v>
       </c>
@@ -43897,8 +43939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C6AE3B-9B6D-42BB-B369-D11B8464ACAE}">
   <dimension ref="A1:AF90"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:AF5"/>
+    <sheetView topLeftCell="P39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X78" sqref="X78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -44429,85 +44471,85 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:32" ht="39.75" customHeight="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="82" t="s">
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="82" t="s">
+      <c r="G4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="82" t="s">
+      <c r="H4" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="82" t="s">
+      <c r="I4" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="84" t="s">
+      <c r="J4" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="84" t="s">
+      <c r="L4" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="84" t="s">
+      <c r="M4" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="84" t="s">
+      <c r="N4" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="84" t="s">
+      <c r="O4" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="86" t="s">
+      <c r="Q4" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="82" t="s">
+      <c r="R4" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="81" t="s">
+      <c r="S4" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81" t="s">
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="95" t="s">
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="95"/>
-      <c r="AB4" s="95" t="s">
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="AC4" s="95"/>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="91" t="s">
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="AF4" s="93" t="s">
+      <c r="AF4" s="86" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="54" customHeight="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="91"/>
       <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
@@ -44517,20 +44559,20 @@
       <c r="D5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="87"/>
-      <c r="R5" s="83"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="97"/>
+      <c r="R5" s="93"/>
       <c r="S5" s="46" t="s">
         <v>16</v>
       </c>
@@ -44567,8 +44609,8 @@
       <c r="AD5" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="AE5" s="92"/>
-      <c r="AF5" s="94"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="87"/>
     </row>
     <row r="6" spans="1:32" ht="15.95" customHeight="1">
       <c r="A6" s="14">
@@ -52260,16 +52302,16 @@
       <c r="R81" s="33"/>
     </row>
     <row r="82" spans="1:18" ht="38.25" customHeight="1">
-      <c r="A82" s="88" t="s">
+      <c r="A82" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="88"/>
-      <c r="C82" s="88"/>
-      <c r="D82" s="88"/>
-      <c r="E82" s="88"/>
-      <c r="F82" s="88"/>
-      <c r="G82" s="88"/>
-      <c r="H82" s="88"/>
+      <c r="B82" s="89"/>
+      <c r="C82" s="89"/>
+      <c r="D82" s="89"/>
+      <c r="E82" s="89"/>
+      <c r="F82" s="89"/>
+      <c r="G82" s="89"/>
+      <c r="H82" s="89"/>
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:18" ht="15.95" customHeight="1">
@@ -52307,18 +52349,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="V4:X4"/>
-    <mergeCell ref="AE4:AE5"/>
-    <mergeCell ref="AF4:AF5"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="A82:H82"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
@@ -52330,6 +52360,18 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="R4:R5"/>
+    <mergeCell ref="A82:H82"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="AE4:AE5"/>
+    <mergeCell ref="AF4:AF5"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -55521,7 +55563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E14718-ED97-474E-9558-AF67D149436E}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
@@ -57859,7 +57901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F3EE34-C2D5-46E7-9B51-5A52C0EB336F}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -59814,10 +59856,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="96"/>
+      <c r="E1" s="98"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="74" t="s">

</xml_diff>